<commit_message>
Initial commit (commit#01): USe the main method in the base class to run the assignment, after refactoring the xcell sheet location.
</commit_message>
<xml_diff>
--- a/qaautomation.xlsx
+++ b/qaautomation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emumba/Desktop/From old PC/Automation Assignment/attemptOne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6130426A-C9BA-374A-B34C-2BFC75AE024B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC9AED4-A4EE-7648-A2A7-7E2B3652DBDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34960" yWindow="3460" windowWidth="28800" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -516,9 +516,6 @@
     <t>Psychiatrist</t>
   </si>
   <si>
-    <t>George</t>
-  </si>
-  <si>
     <t>Roxy</t>
   </si>
   <si>
@@ -825,7 +822,10 @@
     <t>1 episode, 2022</t>
   </si>
   <si>
-    <t>tony.knowstheway1@gmail.com</t>
+    <t>George Braden</t>
+  </si>
+  <si>
+    <t>tony.knowstheway321@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1240,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1775,7 +1775,7 @@
         <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1786,7 +1786,7 @@
         <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1797,7 +1797,7 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1808,7 +1808,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1819,7 +1819,7 @@
         <v>147</v>
       </c>
       <c r="C7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1830,7 +1830,7 @@
         <v>148</v>
       </c>
       <c r="C8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1841,7 +1841,7 @@
         <v>149</v>
       </c>
       <c r="C9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1852,7 +1852,7 @@
         <v>150</v>
       </c>
       <c r="C10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1863,7 +1863,7 @@
         <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1874,7 +1874,7 @@
         <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1885,7 +1885,7 @@
         <v>153</v>
       </c>
       <c r="C13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1896,7 +1896,7 @@
         <v>154</v>
       </c>
       <c r="C14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1907,7 +1907,7 @@
         <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1918,7 +1918,7 @@
         <v>156</v>
       </c>
       <c r="C16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1929,7 +1929,7 @@
         <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1940,7 +1940,7 @@
         <v>158</v>
       </c>
       <c r="C18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1948,10 +1948,10 @@
         <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>261</v>
       </c>
       <c r="C19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1959,10 +1959,10 @@
         <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1970,10 +1970,10 @@
         <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1981,10 +1981,10 @@
         <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1992,10 +1992,10 @@
         <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2003,10 +2003,10 @@
         <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2014,10 +2014,10 @@
         <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2025,10 +2025,10 @@
         <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2036,10 +2036,10 @@
         <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2047,10 +2047,10 @@
         <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2058,10 +2058,10 @@
         <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2069,10 +2069,10 @@
         <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2080,10 +2080,10 @@
         <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2091,10 +2091,10 @@
         <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2102,10 +2102,10 @@
         <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C33" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2113,10 +2113,10 @@
         <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C34" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2124,10 +2124,10 @@
         <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C35" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2135,10 +2135,10 @@
         <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C36" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2146,10 +2146,10 @@
         <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C37" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2157,10 +2157,10 @@
         <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2168,10 +2168,10 @@
         <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C39" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2179,10 +2179,10 @@
         <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2190,10 +2190,10 @@
         <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C41" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2201,10 +2201,10 @@
         <v>92</v>
       </c>
       <c r="B42" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C42" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2212,7 +2212,7 @@
         <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
@@ -2223,7 +2223,7 @@
         <v>94</v>
       </c>
       <c r="B44" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
@@ -2234,7 +2234,7 @@
         <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
@@ -2245,7 +2245,7 @@
         <v>96</v>
       </c>
       <c r="B46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
@@ -2256,7 +2256,7 @@
         <v>97</v>
       </c>
       <c r="B47" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
@@ -2267,10 +2267,10 @@
         <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2278,10 +2278,10 @@
         <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2289,7 +2289,7 @@
         <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C50" t="s">
         <v>17</v>
@@ -2300,10 +2300,10 @@
         <v>101</v>
       </c>
       <c r="B51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C51" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2311,10 +2311,10 @@
         <v>102</v>
       </c>
       <c r="B52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C52" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2322,7 +2322,7 @@
         <v>103</v>
       </c>
       <c r="B53" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C53" t="s">
         <v>17</v>
@@ -2333,7 +2333,7 @@
         <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C54" t="s">
         <v>17</v>
@@ -2344,7 +2344,7 @@
         <v>105</v>
       </c>
       <c r="B55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C55" t="s">
         <v>17</v>
@@ -2355,10 +2355,10 @@
         <v>106</v>
       </c>
       <c r="B56" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C56" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2366,10 +2366,10 @@
         <v>107</v>
       </c>
       <c r="B57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C57" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2377,7 +2377,7 @@
         <v>108</v>
       </c>
       <c r="B58" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C58" t="s">
         <v>17</v>
@@ -2388,7 +2388,7 @@
         <v>109</v>
       </c>
       <c r="B59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C59" t="s">
         <v>17</v>
@@ -2399,7 +2399,7 @@
         <v>110</v>
       </c>
       <c r="B60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C60" t="s">
         <v>17</v>
@@ -2410,7 +2410,7 @@
         <v>111</v>
       </c>
       <c r="B61" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C61" t="s">
         <v>17</v>
@@ -2421,10 +2421,10 @@
         <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C62" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2432,10 +2432,10 @@
         <v>113</v>
       </c>
       <c r="B63" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C63" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2443,10 +2443,10 @@
         <v>114</v>
       </c>
       <c r="B64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C64" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2454,7 +2454,7 @@
         <v>115</v>
       </c>
       <c r="B65" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C65" t="s">
         <v>17</v>
@@ -2465,7 +2465,7 @@
         <v>116</v>
       </c>
       <c r="B66" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C66" t="s">
         <v>17</v>
@@ -2476,10 +2476,10 @@
         <v>117</v>
       </c>
       <c r="B67" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C67" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -2487,7 +2487,7 @@
         <v>118</v>
       </c>
       <c r="B68" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C68" t="s">
         <v>17</v>
@@ -2498,10 +2498,10 @@
         <v>119</v>
       </c>
       <c r="B69" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C69" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -2509,10 +2509,10 @@
         <v>120</v>
       </c>
       <c r="B70" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C70" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -2520,10 +2520,10 @@
         <v>121</v>
       </c>
       <c r="B71" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C71" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -2531,10 +2531,10 @@
         <v>122</v>
       </c>
       <c r="B72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C72" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
@@ -2542,7 +2542,7 @@
         <v>123</v>
       </c>
       <c r="B73" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C73" t="s">
         <v>17</v>
@@ -2553,10 +2553,10 @@
         <v>124</v>
       </c>
       <c r="B74" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C74" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
@@ -2564,10 +2564,10 @@
         <v>125</v>
       </c>
       <c r="B75" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C75" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -2575,10 +2575,10 @@
         <v>126</v>
       </c>
       <c r="B76" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C76" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
@@ -2586,10 +2586,10 @@
         <v>127</v>
       </c>
       <c r="B77" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C77" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
@@ -2597,10 +2597,10 @@
         <v>128</v>
       </c>
       <c r="B78" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C78" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
@@ -2608,10 +2608,10 @@
         <v>129</v>
       </c>
       <c r="B79" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C79" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -2619,10 +2619,10 @@
         <v>130</v>
       </c>
       <c r="B80" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C80" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -2630,10 +2630,10 @@
         <v>131</v>
       </c>
       <c r="B81" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C81" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -2641,10 +2641,10 @@
         <v>132</v>
       </c>
       <c r="B82" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C82" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -2652,10 +2652,10 @@
         <v>133</v>
       </c>
       <c r="B83" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C83" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -2663,10 +2663,10 @@
         <v>134</v>
       </c>
       <c r="B84" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C84" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
@@ -2674,10 +2674,10 @@
         <v>135</v>
       </c>
       <c r="B85" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C85" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
@@ -2685,7 +2685,7 @@
         <v>136</v>
       </c>
       <c r="B86" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C86" t="s">
         <v>17</v>
@@ -2696,7 +2696,7 @@
         <v>137</v>
       </c>
       <c r="B87" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C87" t="s">
         <v>17</v>
@@ -2707,10 +2707,10 @@
         <v>138</v>
       </c>
       <c r="B88" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C88" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
@@ -2718,7 +2718,7 @@
         <v>12</v>
       </c>
       <c r="B89" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C89" t="s">
         <v>17</v>
@@ -2729,7 +2729,7 @@
         <v>11</v>
       </c>
       <c r="B90" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C90" t="s">
         <v>17</v>
@@ -2740,7 +2740,7 @@
         <v>139</v>
       </c>
       <c r="B91" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C91" t="s">
         <v>17</v>
@@ -2751,7 +2751,7 @@
         <v>13</v>
       </c>
       <c r="B92" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C92" t="s">
         <v>17</v>
@@ -2762,10 +2762,10 @@
         <v>140</v>
       </c>
       <c r="B93" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C93" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
@@ -2773,10 +2773,10 @@
         <v>141</v>
       </c>
       <c r="B94" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C94" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
@@ -2784,10 +2784,10 @@
         <v>142</v>
       </c>
       <c r="B95" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C95" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -2795,10 +2795,10 @@
         <v>143</v>
       </c>
       <c r="B96" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C96" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
@@ -2806,10 +2806,10 @@
         <v>144</v>
       </c>
       <c r="B97" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C97" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>